<commit_message>
Fixed parts orientation in PnP file.
</commit_message>
<xml_diff>
--- a/cam/LED-mini-SHIM_2021-05-13-PnP.xlsx
+++ b/cam/LED-mini-SHIM_2021-05-13-PnP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\LED-SHIM\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B9E786-4C9F-4FB6-AD0B-0E1F78FAF645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935E695F-B7E2-4B15-A967-C96A7AE1D084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="550" windowWidth="16430" windowHeight="19950" xr2:uid="{E3D24A52-6DBC-4B10-AB0F-CBBE651E3B98}"/>
+    <workbookView xWindow="24130" yWindow="780" windowWidth="16430" windowHeight="19950" xr2:uid="{E3D24A52-6DBC-4B10-AB0F-CBBE651E3B98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -222,8 +222,8 @@
     <tableColumn id="7" xr3:uid="{AD1FA465-9FA2-4E63-B538-C6C661E1BB55}" uniqueName="7" name="Designator" queryTableFieldId="1" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F2386B6B-12F2-4A2F-A43D-CD55FD88F018}" uniqueName="2" name="Mid X" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{3967EC58-D6BA-4079-A4B1-230DE6CAF157}" uniqueName="3" name="Mid Y" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{F7C560F7-5586-42A7-84CC-9F11E0341A31}" uniqueName="8" name="Layer" queryTableFieldId="7" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{15C5BF37-0177-474D-85BC-A812617A503A}" uniqueName="4" name="Rotation" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{F7C560F7-5586-42A7-84CC-9F11E0341A31}" uniqueName="8" name="Layer" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{15C5BF37-0177-474D-85BC-A812617A503A}" uniqueName="4" name="Rotation" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +570,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -587,7 +587,7 @@
         <v>27</v>
       </c>
       <c r="E3" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -604,7 +604,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -621,7 +621,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,7 +638,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -655,7 +655,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -672,7 +672,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -689,7 +689,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -706,7 +706,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -723,7 +723,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,7 +740,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -757,7 +757,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -774,7 +774,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -791,7 +791,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -825,7 +825,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -842,7 +842,7 @@
         <v>27</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -859,7 +859,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -876,7 +876,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -893,7 +893,7 @@
         <v>27</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -910,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -927,7 +927,7 @@
         <v>27</v>
       </c>
       <c r="E23" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>